<commit_message>
fix values in fixture
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.35.raredisease.xlsx
+++ b/tests/fixtures/orderforms/1508.35.raredisease.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsdiazboada/Documents/Clinical_Genomics/repos/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A6DB50-AE0E-6148-9A35-141B8CE562AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0A6341-4464-6142-91A8-A82271531AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-13500" windowWidth="60160" windowHeight="33360" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="836">
   <si>
     <t>https://clinical.scilifelab.se/</t>
   </si>
@@ -3392,12 +3392,6 @@
     <t>MIP DNA</t>
   </si>
   <si>
-    <t>mipdnasample2</t>
-  </si>
-  <si>
-    <t>mipdnasample3</t>
-  </si>
-  <si>
     <t>rdsample1</t>
   </si>
   <si>
@@ -3642,12 +3636,6 @@
   </si>
   <si>
     <t>rdcase40</t>
-  </si>
-  <si>
-    <t>rdcase41</t>
-  </si>
-  <si>
-    <t>rdcase42</t>
   </si>
   <si>
     <t>rdsubject1</t>
@@ -5982,8 +5970,8 @@
   </sheetPr>
   <dimension ref="A1:AMM395"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -13633,7 +13621,7 @@
     </row>
     <row r="15" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="65" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B15" s="66" t="s">
         <v>66</v>
@@ -13645,7 +13633,7 @@
         <v>451</v>
       </c>
       <c r="E15" s="67" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="F15" s="67" t="s">
         <v>563</v>
@@ -13669,14 +13657,14 @@
         <v>20</v>
       </c>
       <c r="M15" s="107" t="s">
-        <v>794</v>
+        <v>790</v>
       </c>
       <c r="N15" s="84" t="s">
         <v>64</v>
       </c>
       <c r="O15" s="49"/>
       <c r="P15" s="70" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="Q15" s="85" t="s">
         <v>72</v>
@@ -13692,10 +13680,10 @@
         <v>70</v>
       </c>
       <c r="W15" s="65" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="X15" s="71" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="Y15" s="72"/>
       <c r="Z15" s="87"/>
@@ -13717,13 +13705,13 @@
         <v>5</v>
       </c>
       <c r="AH15" s="70" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="AI15" s="88">
         <v>10</v>
       </c>
       <c r="AJ15" s="70" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="AK15"/>
       <c r="AL15"/>
@@ -14718,7 +14706,7 @@
     </row>
     <row r="16" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="65" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B16" s="66" t="s">
         <v>66</v>
@@ -14730,7 +14718,7 @@
         <v>451</v>
       </c>
       <c r="E16" s="67" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="F16" s="67" t="s">
         <v>563</v>
@@ -14754,7 +14742,7 @@
         <v>21</v>
       </c>
       <c r="M16" s="107" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="N16" s="84" t="s">
         <v>74</v>
@@ -15783,7 +15771,7 @@
     </row>
     <row r="17" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="65" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B17" s="66" t="s">
         <v>66</v>
@@ -15795,7 +15783,7 @@
         <v>451</v>
       </c>
       <c r="E17" s="67" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="F17" s="67" t="s">
         <v>563</v>
@@ -15819,7 +15807,7 @@
         <v>22</v>
       </c>
       <c r="M17" s="107" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="N17" s="84" t="s">
         <v>74</v>
@@ -16844,7 +16832,7 @@
     </row>
     <row r="18" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="65" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B18" s="66" t="s">
         <v>66</v>
@@ -16856,7 +16844,7 @@
         <v>451</v>
       </c>
       <c r="E18" s="67" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="F18" s="67" t="s">
         <v>563</v>
@@ -16880,7 +16868,7 @@
         <v>23</v>
       </c>
       <c r="M18" s="107" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="N18" s="84" t="s">
         <v>74</v>
@@ -17905,7 +17893,7 @@
     </row>
     <row r="19" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="65" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B19" s="66" t="s">
         <v>66</v>
@@ -17917,7 +17905,7 @@
         <v>451</v>
       </c>
       <c r="E19" s="67" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="F19" s="67" t="s">
         <v>564</v>
@@ -17941,7 +17929,7 @@
         <v>24</v>
       </c>
       <c r="M19" s="107" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="N19" s="84" t="s">
         <v>74</v>
@@ -18966,7 +18954,7 @@
     </row>
     <row r="20" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="65" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B20" s="66" t="s">
         <v>66</v>
@@ -18978,7 +18966,7 @@
         <v>451</v>
       </c>
       <c r="E20" s="67" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="F20" s="67" t="s">
         <v>564</v>
@@ -19002,7 +18990,7 @@
         <v>25</v>
       </c>
       <c r="M20" s="107" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="N20" s="84" t="s">
         <v>74</v>
@@ -20027,7 +20015,7 @@
     </row>
     <row r="21" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="65" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B21" s="66" t="s">
         <v>66</v>
@@ -20039,7 +20027,7 @@
         <v>451</v>
       </c>
       <c r="E21" s="67" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="F21" s="67" t="s">
         <v>564</v>
@@ -20063,7 +20051,7 @@
         <v>26</v>
       </c>
       <c r="M21" s="107" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
       <c r="N21" s="84" t="s">
         <v>74</v>
@@ -21088,7 +21076,7 @@
     </row>
     <row r="22" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="65" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B22" s="66" t="s">
         <v>66</v>
@@ -21100,7 +21088,7 @@
         <v>451</v>
       </c>
       <c r="E22" s="67" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="F22" s="67" t="s">
         <v>565</v>
@@ -21124,7 +21112,7 @@
         <v>27</v>
       </c>
       <c r="M22" s="107" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="N22" s="84" t="s">
         <v>74</v>
@@ -22149,7 +22137,7 @@
     </row>
     <row r="23" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="65" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B23" s="66" t="s">
         <v>66</v>
@@ -22161,7 +22149,7 @@
         <v>451</v>
       </c>
       <c r="E23" s="67" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="F23" s="67" t="s">
         <v>564</v>
@@ -22185,7 +22173,7 @@
         <v>28</v>
       </c>
       <c r="M23" s="107" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="N23" s="84" t="s">
         <v>74</v>
@@ -23210,7 +23198,7 @@
     </row>
     <row r="24" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="65" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B24" s="66" t="s">
         <v>66</v>
@@ -23222,7 +23210,7 @@
         <v>451</v>
       </c>
       <c r="E24" s="67" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="F24" s="67" t="s">
         <v>564</v>
@@ -23246,7 +23234,7 @@
         <v>29</v>
       </c>
       <c r="M24" s="107" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="N24" s="84" t="s">
         <v>74</v>
@@ -24271,7 +24259,7 @@
     </row>
     <row r="25" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="65" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B25" s="66" t="s">
         <v>66</v>
@@ -24283,7 +24271,7 @@
         <v>451</v>
       </c>
       <c r="E25" s="67" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="F25" s="67" t="s">
         <v>564</v>
@@ -24307,7 +24295,7 @@
         <v>30</v>
       </c>
       <c r="M25" s="107" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="N25" s="84" t="s">
         <v>74</v>
@@ -25332,7 +25320,7 @@
     </row>
     <row r="26" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="65" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="B26" s="66" t="s">
         <v>66</v>
@@ -25344,7 +25332,7 @@
         <v>451</v>
       </c>
       <c r="E26" s="67" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="F26" s="67" t="s">
         <v>565</v>
@@ -25368,7 +25356,7 @@
         <v>31</v>
       </c>
       <c r="M26" s="107" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="N26" s="84" t="s">
         <v>74</v>
@@ -26393,7 +26381,7 @@
     </row>
     <row r="27" spans="1:1026" s="75" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="65" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="B27" s="66" t="s">
         <v>66</v>
@@ -26405,7 +26393,7 @@
         <v>451</v>
       </c>
       <c r="E27" s="67" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="F27" s="67" t="s">
         <v>122</v>
@@ -26429,7 +26417,7 @@
         <v>32</v>
       </c>
       <c r="M27" s="107" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="N27" s="84" t="s">
         <v>74</v>
@@ -26465,7 +26453,7 @@
     </row>
     <row r="28" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="65" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B28" s="66" t="s">
         <v>66</v>
@@ -26477,7 +26465,7 @@
         <v>451</v>
       </c>
       <c r="E28" s="67" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="F28" s="67" t="s">
         <v>122</v>
@@ -26501,7 +26489,7 @@
         <v>33</v>
       </c>
       <c r="M28" s="107" t="s">
-        <v>807</v>
+        <v>803</v>
       </c>
       <c r="N28" s="84" t="s">
         <v>74</v>
@@ -27526,7 +27514,7 @@
     </row>
     <row r="29" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="65" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B29" s="66" t="s">
         <v>66</v>
@@ -27538,7 +27526,7 @@
         <v>451</v>
       </c>
       <c r="E29" s="67" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="F29" s="67" t="s">
         <v>127</v>
@@ -27562,7 +27550,7 @@
         <v>34</v>
       </c>
       <c r="M29" s="107" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="N29" s="84" t="s">
         <v>74</v>
@@ -28587,7 +28575,7 @@
     </row>
     <row r="30" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="65" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="B30" s="66" t="s">
         <v>66</v>
@@ -28599,7 +28587,7 @@
         <v>451</v>
       </c>
       <c r="E30" s="67" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
       <c r="F30" s="67" t="s">
         <v>136</v>
@@ -28611,7 +28599,7 @@
         <v>67</v>
       </c>
       <c r="I30" s="82" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="J30" s="83" t="s">
         <v>93</v>
@@ -28623,7 +28611,7 @@
         <v>35</v>
       </c>
       <c r="M30" s="107" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="N30" s="84" t="s">
         <v>74</v>
@@ -29648,7 +29636,7 @@
     </row>
     <row r="31" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="65" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B31" s="66" t="s">
         <v>66</v>
@@ -29660,7 +29648,7 @@
         <v>451</v>
       </c>
       <c r="E31" s="67" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="F31" s="67" t="s">
         <v>144</v>
@@ -29684,7 +29672,7 @@
         <v>36</v>
       </c>
       <c r="M31" s="107" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="N31" s="84" t="s">
         <v>74</v>
@@ -30709,7 +30697,7 @@
     </row>
     <row r="32" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="65" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B32" s="66" t="s">
         <v>66</v>
@@ -30721,7 +30709,7 @@
         <v>451</v>
       </c>
       <c r="E32" s="67" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="F32" s="67" t="s">
         <v>497</v>
@@ -30745,7 +30733,7 @@
         <v>37</v>
       </c>
       <c r="M32" s="107" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="N32" s="84" t="s">
         <v>74</v>
@@ -31770,7 +31758,7 @@
     </row>
     <row r="33" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="65" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B33" s="66" t="s">
         <v>66</v>
@@ -31782,7 +31770,7 @@
         <v>451</v>
       </c>
       <c r="E33" s="67" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="F33" s="67" t="s">
         <v>144</v>
@@ -31806,7 +31794,7 @@
         <v>38</v>
       </c>
       <c r="M33" s="107" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="N33" s="84" t="s">
         <v>74</v>
@@ -32831,7 +32819,7 @@
     </row>
     <row r="34" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="65" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B34" s="66" t="s">
         <v>66</v>
@@ -32843,7 +32831,7 @@
         <v>451</v>
       </c>
       <c r="E34" s="67" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="F34" s="67" t="s">
         <v>122</v>
@@ -32867,7 +32855,7 @@
         <v>39</v>
       </c>
       <c r="M34" s="107" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="N34" s="84" t="s">
         <v>74</v>
@@ -33892,7 +33880,7 @@
     </row>
     <row r="35" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="65" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B35" s="66" t="s">
         <v>66</v>
@@ -33904,7 +33892,7 @@
         <v>451</v>
       </c>
       <c r="E35" s="67" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="F35" s="67" t="s">
         <v>127</v>
@@ -33928,7 +33916,7 @@
         <v>40</v>
       </c>
       <c r="M35" s="107" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="N35" s="84" t="s">
         <v>74</v>
@@ -34953,7 +34941,7 @@
     </row>
     <row r="36" spans="1:1026" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="65" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B36" s="66" t="s">
         <v>66</v>
@@ -34965,7 +34953,7 @@
         <v>451</v>
       </c>
       <c r="E36" s="67" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="F36" s="67" t="s">
         <v>136</v>
@@ -34989,7 +34977,7 @@
         <v>41</v>
       </c>
       <c r="M36" s="107" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="N36" s="84" t="s">
         <v>74</v>
@@ -35025,7 +35013,7 @@
     </row>
     <row r="37" spans="1:1026" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="65" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B37" s="66" t="s">
         <v>66</v>
@@ -35037,7 +35025,7 @@
         <v>451</v>
       </c>
       <c r="E37" s="67" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="F37" s="67" t="s">
         <v>144</v>
@@ -35061,7 +35049,7 @@
         <v>42</v>
       </c>
       <c r="M37" s="107" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="N37" s="84" t="s">
         <v>74</v>
@@ -35097,7 +35085,7 @@
     </row>
     <row r="38" spans="1:1026" s="76" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="65" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B38" s="66" t="s">
         <v>66</v>
@@ -35109,7 +35097,7 @@
         <v>451</v>
       </c>
       <c r="E38" s="67" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="F38" s="67" t="s">
         <v>497</v>
@@ -35133,7 +35121,7 @@
         <v>43</v>
       </c>
       <c r="M38" s="107" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="N38" s="84" t="s">
         <v>74</v>
@@ -35169,7 +35157,7 @@
     </row>
     <row r="39" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="65" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B39" s="66" t="s">
         <v>66</v>
@@ -35181,7 +35169,7 @@
         <v>451</v>
       </c>
       <c r="E39" s="67" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="F39" s="67" t="s">
         <v>122</v>
@@ -35205,7 +35193,7 @@
         <v>44</v>
       </c>
       <c r="M39" s="107" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="N39" s="84" t="s">
         <v>74</v>
@@ -36230,7 +36218,7 @@
     </row>
     <row r="40" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="65" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B40" s="66" t="s">
         <v>66</v>
@@ -36242,7 +36230,7 @@
         <v>451</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="F40" s="67" t="s">
         <v>127</v>
@@ -36266,7 +36254,7 @@
         <v>45</v>
       </c>
       <c r="M40" s="107" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="N40" s="84" t="s">
         <v>74</v>
@@ -37291,7 +37279,7 @@
     </row>
     <row r="41" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="65" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B41" s="66" t="s">
         <v>66</v>
@@ -37303,7 +37291,7 @@
         <v>451</v>
       </c>
       <c r="E41" s="67" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="F41" s="67" t="s">
         <v>136</v>
@@ -37327,7 +37315,7 @@
         <v>46</v>
       </c>
       <c r="M41" s="107" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="N41" s="84" t="s">
         <v>74</v>
@@ -38352,7 +38340,7 @@
     </row>
     <row r="42" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="65" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B42" s="66" t="s">
         <v>66</v>
@@ -38364,7 +38352,7 @@
         <v>451</v>
       </c>
       <c r="E42" s="67" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="F42" s="67" t="s">
         <v>144</v>
@@ -38388,7 +38376,7 @@
         <v>47</v>
       </c>
       <c r="M42" s="107" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="N42" s="84" t="s">
         <v>74</v>
@@ -39413,7 +39401,7 @@
     </row>
     <row r="43" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="65" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B43" s="66" t="s">
         <v>66</v>
@@ -39425,7 +39413,7 @@
         <v>451</v>
       </c>
       <c r="E43" s="67" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="F43" s="67" t="s">
         <v>497</v>
@@ -39449,7 +39437,7 @@
         <v>48</v>
       </c>
       <c r="M43" s="107" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="N43" s="84" t="s">
         <v>74</v>
@@ -40474,7 +40462,7 @@
     </row>
     <row r="44" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="65" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B44" s="66" t="s">
         <v>66</v>
@@ -40486,7 +40474,7 @@
         <v>451</v>
       </c>
       <c r="E44" s="67" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="F44" s="67" t="s">
         <v>122</v>
@@ -40510,7 +40498,7 @@
         <v>49</v>
       </c>
       <c r="M44" s="107" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="N44" s="84" t="s">
         <v>74</v>
@@ -41535,7 +41523,7 @@
     </row>
     <row r="45" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="65" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B45" s="66" t="s">
         <v>66</v>
@@ -41547,7 +41535,7 @@
         <v>451</v>
       </c>
       <c r="E45" s="67" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="F45" s="67" t="s">
         <v>127</v>
@@ -41571,7 +41559,7 @@
         <v>50</v>
       </c>
       <c r="M45" s="107" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="N45" s="84" t="s">
         <v>74</v>
@@ -42596,7 +42584,7 @@
     </row>
     <row r="46" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="65" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B46" s="66" t="s">
         <v>66</v>
@@ -42608,7 +42596,7 @@
         <v>451</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="F46" s="67" t="s">
         <v>136</v>
@@ -42632,7 +42620,7 @@
         <v>51</v>
       </c>
       <c r="M46" s="107" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="N46" s="84" t="s">
         <v>74</v>
@@ -43657,7 +43645,7 @@
     </row>
     <row r="47" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="65" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B47" s="66" t="s">
         <v>66</v>
@@ -43669,7 +43657,7 @@
         <v>451</v>
       </c>
       <c r="E47" s="67" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="F47" s="67" t="s">
         <v>144</v>
@@ -43693,7 +43681,7 @@
         <v>52</v>
       </c>
       <c r="M47" s="107" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="N47" s="84" t="s">
         <v>74</v>
@@ -44718,7 +44706,7 @@
     </row>
     <row r="48" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="65" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B48" s="66" t="s">
         <v>66</v>
@@ -44730,7 +44718,7 @@
         <v>451</v>
       </c>
       <c r="E48" s="67" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="F48" s="67" t="s">
         <v>497</v>
@@ -44754,7 +44742,7 @@
         <v>53</v>
       </c>
       <c r="M48" s="107" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="N48" s="84" t="s">
         <v>74</v>
@@ -45779,7 +45767,7 @@
     </row>
     <row r="49" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="65" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B49" s="66" t="s">
         <v>66</v>
@@ -45791,7 +45779,7 @@
         <v>451</v>
       </c>
       <c r="E49" s="67" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="F49" s="67" t="s">
         <v>122</v>
@@ -45815,7 +45803,7 @@
         <v>54</v>
       </c>
       <c r="M49" s="107" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="N49" s="84" t="s">
         <v>74</v>
@@ -46840,7 +46828,7 @@
     </row>
     <row r="50" spans="1:1026" s="78" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="77" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B50" s="66" t="s">
         <v>66</v>
@@ -46852,7 +46840,7 @@
         <v>451</v>
       </c>
       <c r="E50" s="67" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="F50" s="67" t="s">
         <v>127</v>
@@ -46876,7 +46864,7 @@
         <v>55</v>
       </c>
       <c r="M50" s="107" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="N50" s="84" t="s">
         <v>74</v>
@@ -46912,7 +46900,7 @@
     </row>
     <row r="51" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="77" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B51" s="66" t="s">
         <v>66</v>
@@ -46924,7 +46912,7 @@
         <v>451</v>
       </c>
       <c r="E51" s="67" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="F51" s="67" t="s">
         <v>136</v>
@@ -46948,7 +46936,7 @@
         <v>56</v>
       </c>
       <c r="M51" s="107" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="N51" s="84" t="s">
         <v>74</v>
@@ -47973,7 +47961,7 @@
     </row>
     <row r="52" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="77" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B52" s="66" t="s">
         <v>66</v>
@@ -47985,7 +47973,7 @@
         <v>451</v>
       </c>
       <c r="E52" s="67" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="F52" s="67" t="s">
         <v>144</v>
@@ -48009,7 +47997,7 @@
         <v>57</v>
       </c>
       <c r="M52" s="107" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="N52" s="84" t="s">
         <v>74</v>
@@ -49034,7 +49022,7 @@
     </row>
     <row r="53" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="77" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B53" s="66" t="s">
         <v>66</v>
@@ -49046,7 +49034,7 @@
         <v>451</v>
       </c>
       <c r="E53" s="67" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="F53" s="67" t="s">
         <v>497</v>
@@ -49070,7 +49058,7 @@
         <v>58</v>
       </c>
       <c r="M53" s="107" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="N53" s="84" t="s">
         <v>74</v>
@@ -50095,7 +50083,7 @@
     </row>
     <row r="54" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="77" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B54" s="66" t="s">
         <v>66</v>
@@ -50107,7 +50095,7 @@
         <v>451</v>
       </c>
       <c r="E54" s="67" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="F54" s="67" t="s">
         <v>122</v>
@@ -50131,7 +50119,7 @@
         <v>59</v>
       </c>
       <c r="M54" s="107" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="N54" s="84" t="s">
         <v>74</v>
@@ -51156,7 +51144,7 @@
     </row>
     <row r="55" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="77" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B55" s="66" t="s">
         <v>66</v>
@@ -51168,7 +51156,7 @@
         <v>451</v>
       </c>
       <c r="E55" s="67" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="F55" s="67" t="s">
         <v>127</v>
@@ -51192,7 +51180,7 @@
         <v>60</v>
       </c>
       <c r="M55" s="107" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="N55" s="84" t="s">
         <v>74</v>
@@ -52217,7 +52205,7 @@
     </row>
     <row r="56" spans="1:1026" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="77" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B56" s="66" t="s">
         <v>66</v>
@@ -52229,7 +52217,7 @@
         <v>451</v>
       </c>
       <c r="E56" s="67" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="F56" s="67" t="s">
         <v>136</v>
@@ -52253,7 +52241,7 @@
         <v>61</v>
       </c>
       <c r="M56" s="107" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="N56" s="84" t="s">
         <v>74</v>
@@ -71910,7 +71898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL313"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -72324,7 +72312,7 @@
         <v>114</v>
       </c>
       <c r="G10" s="123" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="M10" s="118" t="s">
         <v>116</v>

</xml_diff>